<commit_message>
updated DCMEX SS so case 2 aerosol has 4 modes
</commit_message>
<xml_diff>
--- a/parcel-modelling/data/Model_inputs_DCMEX.xlsx
+++ b/parcel-modelling/data/Model_inputs_DCMEX.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11008"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11127"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mccikpc2/Dropbox (Personal)/programming/teaching-repos/projects-and-teaching/parcel-modelling/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E71D9941-51A6-5849-B766-6CC1AF155260}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C26F0C8-9495-2542-AD36-B510B9818A17}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="13040" xr2:uid="{894127C6-20C5-4B29-9E35-433370B386C8}"/>
+    <workbookView xWindow="6400" yWindow="500" windowWidth="31140" windowHeight="17640" xr2:uid="{894127C6-20C5-4B29-9E35-433370B386C8}"/>
   </bookViews>
   <sheets>
     <sheet name="sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="25">
   <si>
     <t>dN/dlnDp</t>
   </si>
@@ -99,6 +99,18 @@
   </si>
   <si>
     <t>Parameters for Case 1</t>
+  </si>
+  <si>
+    <t>n_aer4</t>
+  </si>
+  <si>
+    <t>d_4</t>
+  </si>
+  <si>
+    <t>lnsig4</t>
+  </si>
+  <si>
+    <t>Parameters for Case 2</t>
   </si>
 </sst>
 </file>
@@ -220,7 +232,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -252,6 +264,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -259,12 +274,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1777,40 +1786,40 @@
                   <c:v>895.7872146505689</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>833.49778157659637</c:v>
+                  <c:v>833.49778157659682</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>746.32247044430858</c:v>
+                  <c:v>746.32247044479209</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>642.37412465037914</c:v>
+                  <c:v>642.37412490179906</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>530.78654172861206</c:v>
+                  <c:v>530.78659897571583</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>428.1462274291045</c:v>
+                  <c:v>428.1520780249167</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>403.41660106339543</c:v>
+                  <c:v>403.67213727244786</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>229.62091679840395</c:v>
+                  <c:v>234.14276790962415</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>156.57549736822082</c:v>
+                  <c:v>188.84328343322974</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>101.81140037751567</c:v>
+                  <c:v>189.78153820908318</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>62.707890466235867</c:v>
+                  <c:v>150.06106151659179</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>36.524529466211739</c:v>
+                  <c:v>66.771865453561816</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>19.97675800626498</c:v>
+                  <c:v>23.400060915912007</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3156,16 +3165,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>57150</xdr:rowOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>584200</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>457200</xdr:colOff>
-      <xdr:row>22</xdr:row>
-      <xdr:rowOff>133350</xdr:rowOff>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>190500</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3192,16 +3201,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>501650</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>120650</xdr:rowOff>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>654050</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>31750</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>527050</xdr:colOff>
-      <xdr:row>22</xdr:row>
-      <xdr:rowOff>6350</xdr:rowOff>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>425450</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>107950</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3526,10 +3535,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0ECA62D5-9912-440B-B476-66EE5BC205DA}">
-  <dimension ref="A1:N42"/>
+  <dimension ref="A1:R42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J5" sqref="J5"/>
+      <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3545,17 +3554,16 @@
     <col min="15" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="32" x14ac:dyDescent="0.2">
-      <c r="A1" s="11" t="s">
+    <row r="1" spans="1:18" ht="32" x14ac:dyDescent="0.2">
+      <c r="A1" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="12"/>
+      <c r="B1" s="13"/>
       <c r="C1" s="3"/>
-      <c r="D1" s="12" t="s">
+      <c r="D1" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="13"/>
-      <c r="F1" s="14"/>
+      <c r="E1" s="14"/>
       <c r="H1" s="4"/>
       <c r="I1" s="9" t="s">
         <v>3</v>
@@ -3576,7 +3584,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A2" s="5" t="s">
         <v>9</v>
       </c>
@@ -3592,7 +3600,7 @@
       <c r="E2" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="F2" s="14" t="s">
+      <c r="F2" s="1" t="s">
         <v>19</v>
       </c>
       <c r="H2" s="5" t="s">
@@ -3617,7 +3625,7 @@
         <v>4863.6099999999997</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A3" s="5">
         <v>2.0585842032181501E-2</v>
       </c>
@@ -3625,7 +3633,7 @@
         <v>52.491199845087074</v>
       </c>
       <c r="C3" s="1">
-        <f>I$5/(SQRT(2*PI())*I$11)*EXP(-(LN(A3/I$8)^2)/(2*I$11^2))+I$6/(SQRT(2*PI())*I$12)*EXP(-(LN(A3/I$9)^2)/(2*I$12^2))+ I$7/(SQRT(2*PI())*I$13)*EXP(-(LN(A3/I$10)^2)/(2*I$13^2))</f>
+        <f>I$5/(SQRT(2*PI())*I$13)*EXP(-(LN(A3/I$9)^2)/(2*I$13^2))+I$6/(SQRT(2*PI())*I$14)*EXP(-(LN(A3/I$10)^2)/(2*I$14^2))+ I$7/(SQRT(2*PI())*I$15)*EXP(-(LN(A3/I$11)^2)/(2*I$15^2))</f>
         <v>10.081198378494602</v>
       </c>
       <c r="D3" s="1">
@@ -3635,7 +3643,7 @@
         <v>117.97051441626058</v>
       </c>
       <c r="F3" s="1">
-        <f>L$5/(SQRT(2*PI())*L$11)*EXP(-(LN(D3/L$8)^2)/(2*L$11^2))+L$6/(SQRT(2*PI())*L$12)*EXP(-(LN(D3/L$9)^2)/(2*L$12^2))+ L$7/(SQRT(2*PI())*L$13)*EXP(-(LN(D3/L$10)^2)/(2*L$13^2))</f>
+        <f>L$5/(SQRT(2*PI())*L$13)*EXP(-(LN(D3/L$9)^2)/(2*L$13^2))+L$6/(SQRT(2*PI())*L$14)*EXP(-(LN(D3/L$10)^2)/(2*L$14^2))+ L$7/(SQRT(2*PI())*L$15)*EXP(-(LN(D3/L$11)^2)/(2*L$15^2))+ L$8/(SQRT(2*PI())*L$16)*EXP(-(LN(D3/L$12)^2)/(2*L$16^2))</f>
         <v>10.934801311788796</v>
       </c>
       <c r="H3" s="6" t="s">
@@ -3660,7 +3668,7 @@
         <v>3947.81</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A4" s="5">
         <v>2.1946105153936999E-2</v>
       </c>
@@ -3668,7 +3676,7 @@
         <v>58.627403511134411</v>
       </c>
       <c r="C4" s="1">
-        <f t="shared" ref="C4:C42" si="0">I$5/(SQRT(2*PI())*I$11)*EXP(-(LN(A4/I$8)^2)/(2*I$11^2))+I$6/(SQRT(2*PI())*I$12)*EXP(-(LN(A4/I$9)^2)/(2*I$12^2))+ I$7/(SQRT(2*PI())*I$13)*EXP(-(LN(A4/I$10)^2)/(2*I$13^2))</f>
+        <f>I$5/(SQRT(2*PI())*I$13)*EXP(-(LN(A4/I$9)^2)/(2*I$13^2))+I$6/(SQRT(2*PI())*I$14)*EXP(-(LN(A4/I$10)^2)/(2*I$14^2))+ I$7/(SQRT(2*PI())*I$15)*EXP(-(LN(A4/I$11)^2)/(2*I$15^2))</f>
         <v>19.259167560279273</v>
       </c>
       <c r="D4" s="1">
@@ -3678,20 +3686,24 @@
         <v>170.48941977279736</v>
       </c>
       <c r="F4" s="1">
-        <f t="shared" ref="F4:F42" si="1">L$5/(SQRT(2*PI())*L$11)*EXP(-(LN(D4/L$8)^2)/(2*L$11^2))+L$6/(SQRT(2*PI())*L$12)*EXP(-(LN(D4/L$9)^2)/(2*L$12^2))+ L$7/(SQRT(2*PI())*L$13)*EXP(-(LN(D4/L$10)^2)/(2*L$13^2))</f>
+        <f t="shared" ref="F4:F42" si="0">L$5/(SQRT(2*PI())*L$13)*EXP(-(LN(D4/L$9)^2)/(2*L$13^2))+L$6/(SQRT(2*PI())*L$14)*EXP(-(LN(D4/L$10)^2)/(2*L$14^2))+ L$7/(SQRT(2*PI())*L$15)*EXP(-(LN(D4/L$11)^2)/(2*L$15^2))+ L$8/(SQRT(2*PI())*L$16)*EXP(-(LN(D4/L$12)^2)/(2*L$16^2))</f>
         <v>20.194973605204581</v>
       </c>
-      <c r="H4" s="15" t="s">
+      <c r="H4" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="I4" s="15"/>
-      <c r="J4" s="15"/>
-      <c r="K4" s="15" t="s">
-        <v>20</v>
-      </c>
-      <c r="L4" s="15"/>
+      <c r="I4" s="11"/>
+      <c r="J4" s="11"/>
+      <c r="K4" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="L4" s="11"/>
+      <c r="R4" s="1">
+        <f>1/(LOG10(10)/LN(10))</f>
+        <v>2.3025850929940459</v>
+      </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A5" s="5">
         <v>2.3399052569740699E-2</v>
       </c>
@@ -3699,7 +3711,7 @@
         <v>108.2491188585342</v>
       </c>
       <c r="C5" s="1">
-        <f t="shared" si="0"/>
+        <f>I$5/(SQRT(2*PI())*I$13)*EXP(-(LN(A5/I$9)^2)/(2*I$13^2))+I$6/(SQRT(2*PI())*I$14)*EXP(-(LN(A5/I$10)^2)/(2*I$14^2))+ I$7/(SQRT(2*PI())*I$15)*EXP(-(LN(A5/I$11)^2)/(2*I$15^2))</f>
         <v>34.530593943896214</v>
       </c>
       <c r="D5" s="1">
@@ -3709,24 +3721,24 @@
         <v>291.21194793063796</v>
       </c>
       <c r="F5" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>35.645150241008942</v>
       </c>
-      <c r="H5" s="15" t="s">
+      <c r="H5" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="I5" s="15">
+      <c r="I5" s="11">
         <v>850</v>
       </c>
-      <c r="J5" s="15"/>
-      <c r="K5" s="15" t="s">
+      <c r="J5" s="11"/>
+      <c r="K5" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="L5" s="15">
+      <c r="L5" s="11">
         <v>850</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A6" s="5">
         <v>2.4950842104460001E-2</v>
       </c>
@@ -3734,7 +3746,7 @@
         <v>89.631163253661228</v>
       </c>
       <c r="C6" s="1">
-        <f t="shared" si="0"/>
+        <f>I$5/(SQRT(2*PI())*I$13)*EXP(-(LN(A6/I$9)^2)/(2*I$13^2))+I$6/(SQRT(2*PI())*I$14)*EXP(-(LN(A6/I$10)^2)/(2*I$14^2))+ I$7/(SQRT(2*PI())*I$15)*EXP(-(LN(A6/I$11)^2)/(2*I$15^2))</f>
         <v>58.084674058209195</v>
       </c>
       <c r="D6" s="1">
@@ -3744,24 +3756,24 @@
         <v>347.51979859310615</v>
       </c>
       <c r="F6" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>60.126940395527484</v>
       </c>
-      <c r="H6" s="15" t="s">
+      <c r="H6" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="I6" s="15">
+      <c r="I6" s="11">
         <v>8</v>
       </c>
-      <c r="J6" s="15"/>
-      <c r="K6" s="15" t="s">
+      <c r="J6" s="11"/>
+      <c r="K6" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="L6" s="15">
+      <c r="L6" s="11">
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A7" s="5">
         <v>2.6609157763029401E-2</v>
       </c>
@@ -3769,7 +3781,7 @@
         <v>159.80066051323647</v>
       </c>
       <c r="C7" s="1">
-        <f t="shared" si="0"/>
+        <f>I$5/(SQRT(2*PI())*I$13)*EXP(-(LN(A7/I$9)^2)/(2*I$13^2))+I$6/(SQRT(2*PI())*I$14)*EXP(-(LN(A7/I$10)^2)/(2*I$14^2))+ I$7/(SQRT(2*PI())*I$15)*EXP(-(LN(A7/I$11)^2)/(2*I$15^2))</f>
         <v>91.678963292810039</v>
       </c>
       <c r="D7" s="1">
@@ -3779,24 +3791,24 @@
         <v>314.00240783437999</v>
       </c>
       <c r="F7" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>96.893526478895026</v>
       </c>
-      <c r="H7" s="15" t="s">
+      <c r="H7" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="I7" s="15">
+      <c r="I7" s="11">
         <v>210</v>
       </c>
-      <c r="J7" s="15"/>
-      <c r="K7" s="15" t="s">
+      <c r="J7" s="11"/>
+      <c r="K7" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="L7" s="15">
+      <c r="L7" s="11">
         <v>650</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A8" s="5">
         <v>2.8381210527921901E-2</v>
       </c>
@@ -3804,7 +3816,7 @@
         <v>188.93773086869186</v>
       </c>
       <c r="C8" s="1">
-        <f t="shared" si="0"/>
+        <f>I$5/(SQRT(2*PI())*I$13)*EXP(-(LN(A8/I$9)^2)/(2*I$13^2))+I$6/(SQRT(2*PI())*I$14)*EXP(-(LN(A8/I$10)^2)/(2*I$14^2))+ I$7/(SQRT(2*PI())*I$15)*EXP(-(LN(A8/I$11)^2)/(2*I$15^2))</f>
         <v>135.77582852185941</v>
       </c>
       <c r="D8" s="1">
@@ -3814,24 +3826,22 @@
         <v>356.79368511686471</v>
       </c>
       <c r="F8" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>149.15416434531954</v>
       </c>
-      <c r="H8" s="15" t="s">
-        <v>13</v>
-      </c>
-      <c r="I8" s="15">
-        <v>9.9000000000000005E-2</v>
-      </c>
-      <c r="J8" s="15"/>
-      <c r="K8" s="15" t="s">
-        <v>13</v>
-      </c>
-      <c r="L8" s="15">
-        <v>0.115</v>
+      <c r="H8" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="I8" s="11"/>
+      <c r="J8" s="11"/>
+      <c r="K8" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="L8" s="11">
+        <v>20</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A9" s="5">
         <v>3.0275631452861499E-2</v>
       </c>
@@ -3839,7 +3849,7 @@
         <v>227.61416095986709</v>
       </c>
       <c r="C9" s="1">
-        <f t="shared" si="0"/>
+        <f>I$5/(SQRT(2*PI())*I$13)*EXP(-(LN(A9/I$9)^2)/(2*I$13^2))+I$6/(SQRT(2*PI())*I$14)*EXP(-(LN(A9/I$10)^2)/(2*I$14^2))+ I$7/(SQRT(2*PI())*I$15)*EXP(-(LN(A9/I$11)^2)/(2*I$15^2))</f>
         <v>188.76761667124666</v>
       </c>
       <c r="D9" s="1">
@@ -3849,24 +3859,24 @@
         <v>415.89535802551353</v>
       </c>
       <c r="F9" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>219.32432278080154</v>
       </c>
-      <c r="H9" s="15" t="s">
-        <v>14</v>
-      </c>
-      <c r="I9" s="15">
-        <v>0.2</v>
-      </c>
-      <c r="J9" s="15"/>
-      <c r="K9" s="15" t="s">
-        <v>14</v>
-      </c>
-      <c r="L9" s="15">
-        <v>0.19500000000000001</v>
+      <c r="H9" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="I9" s="11">
+        <v>9.9000000000000005E-2</v>
+      </c>
+      <c r="J9" s="11"/>
+      <c r="K9" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="L9" s="11">
+        <v>0.115</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A10" s="5">
         <v>3.2304526078073603E-2</v>
       </c>
@@ -3874,7 +3884,7 @@
         <v>200.89282579307707</v>
       </c>
       <c r="C10" s="1">
-        <f t="shared" si="0"/>
+        <f>I$5/(SQRT(2*PI())*I$13)*EXP(-(LN(A10/I$9)^2)/(2*I$13^2))+I$6/(SQRT(2*PI())*I$14)*EXP(-(LN(A10/I$10)^2)/(2*I$14^2))+ I$7/(SQRT(2*PI())*I$15)*EXP(-(LN(A10/I$11)^2)/(2*I$15^2))</f>
         <v>246.65874362085773</v>
       </c>
       <c r="D10" s="1">
@@ -3884,24 +3894,24 @@
         <v>447.54847540985884</v>
       </c>
       <c r="F10" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>308.05030355286721</v>
       </c>
-      <c r="H10" s="15" t="s">
-        <v>15</v>
-      </c>
-      <c r="I10" s="15">
-        <v>0.04</v>
-      </c>
-      <c r="J10" s="15"/>
-      <c r="K10" s="15" t="s">
-        <v>15</v>
-      </c>
-      <c r="L10" s="15">
-        <v>0.05</v>
+      <c r="H10" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="I10" s="11">
+        <v>0.2</v>
+      </c>
+      <c r="J10" s="11"/>
+      <c r="K10" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="L10" s="11">
+        <v>0.19500000000000001</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A11" s="5">
         <v>3.4482052250912297E-2</v>
       </c>
@@ -3909,7 +3919,7 @@
         <v>326.14038913582755</v>
       </c>
       <c r="C11" s="1">
-        <f t="shared" si="0"/>
+        <f>I$5/(SQRT(2*PI())*I$13)*EXP(-(LN(A11/I$9)^2)/(2*I$13^2))+I$6/(SQRT(2*PI())*I$14)*EXP(-(LN(A11/I$10)^2)/(2*I$14^2))+ I$7/(SQRT(2*PI())*I$15)*EXP(-(LN(A11/I$11)^2)/(2*I$15^2))</f>
         <v>303.40212828712856</v>
       </c>
       <c r="D11" s="1">
@@ -3919,24 +3929,24 @@
         <v>651.00146462544615</v>
       </c>
       <c r="F11" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>413.25035628312082</v>
       </c>
-      <c r="H11" s="15" t="s">
-        <v>16</v>
-      </c>
-      <c r="I11" s="15">
-        <v>0.39</v>
-      </c>
-      <c r="J11" s="15"/>
-      <c r="K11" s="15" t="s">
-        <v>16</v>
-      </c>
-      <c r="L11" s="15">
-        <v>0.37</v>
+      <c r="H11" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="I11" s="11">
+        <v>0.04</v>
+      </c>
+      <c r="J11" s="11"/>
+      <c r="K11" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="L11" s="11">
+        <v>0.05</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A12" s="5">
         <v>3.6800105647036903E-2</v>
       </c>
@@ -3944,7 +3954,7 @@
         <v>305.07531009150398</v>
       </c>
       <c r="C12" s="1">
-        <f t="shared" si="0"/>
+        <f>I$5/(SQRT(2*PI())*I$13)*EXP(-(LN(A12/I$9)^2)/(2*I$13^2))+I$6/(SQRT(2*PI())*I$14)*EXP(-(LN(A12/I$10)^2)/(2*I$14^2))+ I$7/(SQRT(2*PI())*I$15)*EXP(-(LN(A12/I$11)^2)/(2*I$15^2))</f>
         <v>351.74355302069472</v>
       </c>
       <c r="D12" s="1">
@@ -3954,24 +3964,22 @@
         <v>645.07934001165256</v>
       </c>
       <c r="F12" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>529.90366726758236</v>
       </c>
-      <c r="H12" s="15" t="s">
-        <v>17</v>
-      </c>
-      <c r="I12" s="15">
-        <v>0.05</v>
-      </c>
-      <c r="J12" s="15"/>
-      <c r="K12" s="15" t="s">
-        <v>17</v>
-      </c>
-      <c r="L12" s="15">
-        <v>0.03</v>
+      <c r="H12" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="I12" s="11"/>
+      <c r="J12" s="11"/>
+      <c r="K12" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="L12" s="11">
+        <v>0.26</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A13" s="5">
         <v>3.9280421206825601E-2</v>
       </c>
@@ -3979,7 +3987,7 @@
         <v>357.75415775246637</v>
       </c>
       <c r="C13" s="1">
-        <f t="shared" si="0"/>
+        <f>I$5/(SQRT(2*PI())*I$13)*EXP(-(LN(A13/I$9)^2)/(2*I$13^2))+I$6/(SQRT(2*PI())*I$14)*EXP(-(LN(A13/I$10)^2)/(2*I$14^2))+ I$7/(SQRT(2*PI())*I$15)*EXP(-(LN(A13/I$11)^2)/(2*I$15^2))</f>
         <v>386.62820400969184</v>
       </c>
       <c r="D13" s="1">
@@ -3989,24 +3997,24 @@
         <v>782.83434432532022</v>
       </c>
       <c r="F13" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>649.25240034801948</v>
       </c>
-      <c r="H13" s="15" t="s">
-        <v>18</v>
-      </c>
-      <c r="I13" s="15">
-        <v>0.25</v>
-      </c>
-      <c r="J13" s="15"/>
-      <c r="K13" s="15" t="s">
-        <v>18</v>
-      </c>
-      <c r="L13" s="15">
-        <v>0.3</v>
+      <c r="H13" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="I13" s="11">
+        <v>0.39</v>
+      </c>
+      <c r="J13" s="11"/>
+      <c r="K13" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="L13" s="11">
+        <v>0.37</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A14" s="5">
         <v>4.1937052275005098E-2</v>
       </c>
@@ -4014,7 +4022,7 @@
         <v>328.96177935428136</v>
       </c>
       <c r="C14" s="1">
-        <f t="shared" si="0"/>
+        <f>I$5/(SQRT(2*PI())*I$13)*EXP(-(LN(A14/I$9)^2)/(2*I$13^2))+I$6/(SQRT(2*PI())*I$14)*EXP(-(LN(A14/I$10)^2)/(2*I$14^2))+ I$7/(SQRT(2*PI())*I$15)*EXP(-(LN(A14/I$11)^2)/(2*I$15^2))</f>
         <v>406.07227531414048</v>
       </c>
       <c r="D14" s="1">
@@ -4024,11 +4032,24 @@
         <v>932.73493073684688</v>
       </c>
       <c r="F14" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>759.89993858758487</v>
       </c>
+      <c r="H14" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="I14" s="11">
+        <v>0.05</v>
+      </c>
+      <c r="J14" s="11"/>
+      <c r="K14" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="L14" s="11">
+        <v>0.03</v>
+      </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A15" s="5">
         <v>4.4783262754741399E-2</v>
       </c>
@@ -4036,7 +4057,7 @@
         <v>422.70865688852854</v>
       </c>
       <c r="C15" s="1">
-        <f t="shared" si="0"/>
+        <f>I$5/(SQRT(2*PI())*I$13)*EXP(-(LN(A15/I$9)^2)/(2*I$13^2))+I$6/(SQRT(2*PI())*I$14)*EXP(-(LN(A15/I$10)^2)/(2*I$14^2))+ I$7/(SQRT(2*PI())*I$15)*EXP(-(LN(A15/I$11)^2)/(2*I$15^2))</f>
         <v>412.45302105196879</v>
       </c>
       <c r="D15" s="1">
@@ -4046,11 +4067,24 @@
         <v>879.12062424279691</v>
       </c>
       <c r="F15" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>851.54833188008809</v>
       </c>
+      <c r="H15" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="I15" s="11">
+        <v>0.25</v>
+      </c>
+      <c r="J15" s="11"/>
+      <c r="K15" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="L15" s="11">
+        <v>0.3</v>
+      </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A16" s="5">
         <v>4.7834526463558798E-2</v>
       </c>
@@ -4058,7 +4092,7 @@
         <v>419.90052891415195</v>
       </c>
       <c r="C16" s="1">
-        <f t="shared" si="0"/>
+        <f>I$5/(SQRT(2*PI())*I$13)*EXP(-(LN(A16/I$9)^2)/(2*I$13^2))+I$6/(SQRT(2*PI())*I$14)*EXP(-(LN(A16/I$10)^2)/(2*I$14^2))+ I$7/(SQRT(2*PI())*I$15)*EXP(-(LN(A16/I$11)^2)/(2*I$15^2))</f>
         <v>412.16913945029182</v>
       </c>
       <c r="D16" s="1">
@@ -4068,8 +4102,19 @@
         <v>902.02102188467734</v>
       </c>
       <c r="F16" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>915.37347690930892</v>
+      </c>
+      <c r="H16" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="I16" s="11"/>
+      <c r="J16" s="11"/>
+      <c r="K16" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="L16" s="11">
+        <v>0.08</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
@@ -4080,7 +4125,7 @@
         <v>446.9985288066797</v>
       </c>
       <c r="C17" s="1">
-        <f t="shared" si="0"/>
+        <f>I$5/(SQRT(2*PI())*I$13)*EXP(-(LN(A17/I$9)^2)/(2*I$13^2))+I$6/(SQRT(2*PI())*I$14)*EXP(-(LN(A17/I$10)^2)/(2*I$14^2))+ I$7/(SQRT(2*PI())*I$15)*EXP(-(LN(A17/I$11)^2)/(2*I$15^2))</f>
         <v>413.87784483827056</v>
       </c>
       <c r="D17" s="1">
@@ -4090,7 +4135,7 @@
         <v>967.71321864072092</v>
       </c>
       <c r="F17" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>946.89683702321406</v>
       </c>
     </row>
@@ -4102,7 +4147,7 @@
         <v>537.06338247850158</v>
       </c>
       <c r="C18" s="1">
-        <f t="shared" si="0"/>
+        <f>I$5/(SQRT(2*PI())*I$13)*EXP(-(LN(A18/I$9)^2)/(2*I$13^2))+I$6/(SQRT(2*PI())*I$14)*EXP(-(LN(A18/I$10)^2)/(2*I$14^2))+ I$7/(SQRT(2*PI())*I$15)*EXP(-(LN(A18/I$11)^2)/(2*I$15^2))</f>
         <v>426.00400577091585</v>
       </c>
       <c r="D18" s="1">
@@ -4112,7 +4157,7 @@
         <v>928.97525087370684</v>
       </c>
       <c r="F18" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>947.3522800143345</v>
       </c>
     </row>
@@ -4124,7 +4169,7 @@
         <v>471.13369799051463</v>
       </c>
       <c r="C19" s="1">
-        <f t="shared" si="0"/>
+        <f>I$5/(SQRT(2*PI())*I$13)*EXP(-(LN(A19/I$9)^2)/(2*I$13^2))+I$6/(SQRT(2*PI())*I$14)*EXP(-(LN(A19/I$10)^2)/(2*I$14^2))+ I$7/(SQRT(2*PI())*I$15)*EXP(-(LN(A19/I$11)^2)/(2*I$15^2))</f>
         <v>454.41664091422081</v>
       </c>
       <c r="D19" s="1">
@@ -4134,7 +4179,7 @@
         <v>815.27941556941141</v>
       </c>
       <c r="F19" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>923.67947725405236</v>
       </c>
     </row>
@@ -4146,7 +4191,7 @@
         <v>564.28615969895327</v>
       </c>
       <c r="C20" s="1">
-        <f t="shared" si="0"/>
+        <f>I$5/(SQRT(2*PI())*I$13)*EXP(-(LN(A20/I$9)^2)/(2*I$13^2))+I$6/(SQRT(2*PI())*I$14)*EXP(-(LN(A20/I$10)^2)/(2*I$14^2))+ I$7/(SQRT(2*PI())*I$15)*EXP(-(LN(A20/I$11)^2)/(2*I$15^2))</f>
         <v>501.0075490579124</v>
       </c>
       <c r="D20" s="1">
@@ -4156,7 +4201,7 @@
         <v>842.06460403468395</v>
       </c>
       <c r="F20" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>887.01489146612448</v>
       </c>
     </row>
@@ -4168,7 +4213,7 @@
         <v>610.34379605917911</v>
       </c>
       <c r="C21" s="1">
-        <f t="shared" si="0"/>
+        <f>I$5/(SQRT(2*PI())*I$13)*EXP(-(LN(A21/I$9)^2)/(2*I$13^2))+I$6/(SQRT(2*PI())*I$14)*EXP(-(LN(A21/I$10)^2)/(2*I$14^2))+ I$7/(SQRT(2*PI())*I$15)*EXP(-(LN(A21/I$11)^2)/(2*I$15^2))</f>
         <v>563.52684483781286</v>
       </c>
       <c r="D21" s="1">
@@ -4178,7 +4223,7 @@
         <v>848.92854901910528</v>
       </c>
       <c r="F21" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>850.05761358945995</v>
       </c>
     </row>
@@ -4190,7 +4235,7 @@
         <v>658.37625772315744</v>
       </c>
       <c r="C22" s="1">
-        <f t="shared" si="0"/>
+        <f>I$5/(SQRT(2*PI())*I$13)*EXP(-(LN(A22/I$9)^2)/(2*I$13^2))+I$6/(SQRT(2*PI())*I$14)*EXP(-(LN(A22/I$10)^2)/(2*I$14^2))+ I$7/(SQRT(2*PI())*I$15)*EXP(-(LN(A22/I$11)^2)/(2*I$15^2))</f>
         <v>636.35780123581549</v>
       </c>
       <c r="D22" s="1">
@@ -4200,7 +4245,7 @@
         <v>760.56818604248417</v>
       </c>
       <c r="F22" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>824.03668041336675</v>
       </c>
     </row>
@@ -4212,7 +4257,7 @@
         <v>706.86823380234512</v>
       </c>
       <c r="C23" s="1">
-        <f t="shared" si="0"/>
+        <f>I$5/(SQRT(2*PI())*I$13)*EXP(-(LN(A23/I$9)^2)/(2*I$13^2))+I$6/(SQRT(2*PI())*I$14)*EXP(-(LN(A23/I$10)^2)/(2*I$14^2))+ I$7/(SQRT(2*PI())*I$15)*EXP(-(LN(A23/I$11)^2)/(2*I$15^2))</f>
         <v>710.84180263220389</v>
       </c>
       <c r="D23" s="1">
@@ -4222,7 +4267,7 @@
         <v>727.53125037423229</v>
       </c>
       <c r="F23" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>816.11172040077304</v>
       </c>
     </row>
@@ -4234,7 +4279,7 @@
         <v>769.78456308614113</v>
       </c>
       <c r="C24" s="1">
-        <f t="shared" si="0"/>
+        <f>I$5/(SQRT(2*PI())*I$13)*EXP(-(LN(A24/I$9)^2)/(2*I$13^2))+I$6/(SQRT(2*PI())*I$14)*EXP(-(LN(A24/I$10)^2)/(2*I$14^2))+ I$7/(SQRT(2*PI())*I$15)*EXP(-(LN(A24/I$11)^2)/(2*I$15^2))</f>
         <v>778.64974130183646</v>
       </c>
       <c r="D24" s="1">
@@ -4244,7 +4289,7 @@
         <v>806.37653772573719</v>
       </c>
       <c r="F24" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>827.95878782324576</v>
       </c>
     </row>
@@ -4256,7 +4301,7 @@
         <v>808.60650804549834</v>
       </c>
       <c r="C25" s="1">
-        <f t="shared" si="0"/>
+        <f>I$5/(SQRT(2*PI())*I$13)*EXP(-(LN(A25/I$9)^2)/(2*I$13^2))+I$6/(SQRT(2*PI())*I$14)*EXP(-(LN(A25/I$10)^2)/(2*I$14^2))+ I$7/(SQRT(2*PI())*I$15)*EXP(-(LN(A25/I$11)^2)/(2*I$15^2))</f>
         <v>831.72923362901929</v>
       </c>
       <c r="D25" s="1">
@@ -4266,7 +4311,7 @@
         <v>862.80393379358952</v>
       </c>
       <c r="F25" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>855.32296089411307</v>
       </c>
     </row>
@@ -4278,7 +4323,7 @@
         <v>933.46434032341369</v>
       </c>
       <c r="C26" s="1">
-        <f t="shared" si="0"/>
+        <f>I$5/(SQRT(2*PI())*I$13)*EXP(-(LN(A26/I$9)^2)/(2*I$13^2))+I$6/(SQRT(2*PI())*I$14)*EXP(-(LN(A26/I$10)^2)/(2*I$14^2))+ I$7/(SQRT(2*PI())*I$15)*EXP(-(LN(A26/I$11)^2)/(2*I$15^2))</f>
         <v>863.11932135941731</v>
       </c>
       <c r="D26" s="1">
@@ -4288,7 +4333,7 @@
         <v>865.61469766168511</v>
       </c>
       <c r="F26" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>889.76956505562646</v>
       </c>
     </row>
@@ -4300,7 +4345,7 @@
         <v>780.79472224801725</v>
       </c>
       <c r="C27" s="1">
-        <f t="shared" si="0"/>
+        <f>I$5/(SQRT(2*PI())*I$13)*EXP(-(LN(A27/I$9)^2)/(2*I$13^2))+I$6/(SQRT(2*PI())*I$14)*EXP(-(LN(A27/I$10)^2)/(2*I$14^2))+ I$7/(SQRT(2*PI())*I$15)*EXP(-(LN(A27/I$11)^2)/(2*I$15^2))</f>
         <v>868.77415789684426</v>
       </c>
       <c r="D27" s="1">
@@ -4310,7 +4355,7 @@
         <v>911.23548347983058</v>
       </c>
       <c r="F27" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>920.55537370546961</v>
       </c>
     </row>
@@ -4322,7 +4367,7 @@
         <v>783.52343720236263</v>
       </c>
       <c r="C28" s="1">
-        <f t="shared" si="0"/>
+        <f>I$5/(SQRT(2*PI())*I$13)*EXP(-(LN(A28/I$9)^2)/(2*I$13^2))+I$6/(SQRT(2*PI())*I$14)*EXP(-(LN(A28/I$10)^2)/(2*I$14^2))+ I$7/(SQRT(2*PI())*I$15)*EXP(-(LN(A28/I$11)^2)/(2*I$15^2))</f>
         <v>846.75086015701879</v>
       </c>
       <c r="D28" s="1">
@@ -4332,7 +4377,7 @@
         <v>886.13116431298579</v>
       </c>
       <c r="F28" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>936.79473853996444</v>
       </c>
     </row>
@@ -4344,7 +4389,7 @@
         <v>810.88672886962422</v>
       </c>
       <c r="C29" s="1">
-        <f t="shared" si="0"/>
+        <f>I$5/(SQRT(2*PI())*I$13)*EXP(-(LN(A29/I$9)^2)/(2*I$13^2))+I$6/(SQRT(2*PI())*I$14)*EXP(-(LN(A29/I$10)^2)/(2*I$14^2))+ I$7/(SQRT(2*PI())*I$15)*EXP(-(LN(A29/I$11)^2)/(2*I$15^2))</f>
         <v>798.3792505150036</v>
       </c>
       <c r="D29" s="1">
@@ -4354,7 +4399,7 @@
         <v>887.25357655022356</v>
       </c>
       <c r="F29" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>930.16621901167389</v>
       </c>
     </row>
@@ -4366,7 +4411,7 @@
         <v>678.64617220438208</v>
       </c>
       <c r="C30" s="1">
-        <f t="shared" si="0"/>
+        <f>I$5/(SQRT(2*PI())*I$13)*EXP(-(LN(A30/I$9)^2)/(2*I$13^2))+I$6/(SQRT(2*PI())*I$14)*EXP(-(LN(A30/I$10)^2)/(2*I$14^2))+ I$7/(SQRT(2*PI())*I$15)*EXP(-(LN(A30/I$11)^2)/(2*I$15^2))</f>
         <v>726.96498871041945</v>
       </c>
       <c r="D30" s="1">
@@ -4376,7 +4421,7 @@
         <v>820.47400049698149</v>
       </c>
       <c r="F30" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>895.7872146505689</v>
       </c>
     </row>
@@ -4388,7 +4433,7 @@
         <v>637.68656013974373</v>
       </c>
       <c r="C31" s="1">
-        <f t="shared" si="0"/>
+        <f>I$5/(SQRT(2*PI())*I$13)*EXP(-(LN(A31/I$9)^2)/(2*I$13^2))+I$6/(SQRT(2*PI())*I$14)*EXP(-(LN(A31/I$10)^2)/(2*I$14^2))+ I$7/(SQRT(2*PI())*I$15)*EXP(-(LN(A31/I$11)^2)/(2*I$15^2))</f>
         <v>638.87902940475726</v>
       </c>
       <c r="D31" s="1">
@@ -4398,8 +4443,8 @@
         <v>835.39375733497491</v>
       </c>
       <c r="F31" s="1">
-        <f t="shared" si="1"/>
-        <v>833.49778157659637</v>
+        <f t="shared" si="0"/>
+        <v>833.49778157659682</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.2">
@@ -4410,7 +4455,7 @@
         <v>550.65214105984353</v>
       </c>
       <c r="C32" s="1">
-        <f t="shared" si="0"/>
+        <f>I$5/(SQRT(2*PI())*I$13)*EXP(-(LN(A32/I$9)^2)/(2*I$13^2))+I$6/(SQRT(2*PI())*I$14)*EXP(-(LN(A32/I$10)^2)/(2*I$14^2))+ I$7/(SQRT(2*PI())*I$15)*EXP(-(LN(A32/I$11)^2)/(2*I$15^2))</f>
         <v>541.35412765162869</v>
       </c>
       <c r="D32" s="1">
@@ -4420,8 +4465,8 @@
         <v>806.45050343147011</v>
       </c>
       <c r="F32" s="1">
-        <f t="shared" si="1"/>
-        <v>746.32247044430858</v>
+        <f t="shared" si="0"/>
+        <v>746.32247044479209</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.2">
@@ -4432,7 +4477,7 @@
         <v>474.75781633206077</v>
       </c>
       <c r="C33" s="1">
-        <f t="shared" si="0"/>
+        <f>I$5/(SQRT(2*PI())*I$13)*EXP(-(LN(A33/I$9)^2)/(2*I$13^2))+I$6/(SQRT(2*PI())*I$14)*EXP(-(LN(A33/I$10)^2)/(2*I$14^2))+ I$7/(SQRT(2*PI())*I$15)*EXP(-(LN(A33/I$11)^2)/(2*I$15^2))</f>
         <v>441.8041486573677</v>
       </c>
       <c r="D33" s="1">
@@ -4442,8 +4487,8 @@
         <v>705.18796255269046</v>
       </c>
       <c r="F33" s="1">
-        <f t="shared" si="1"/>
-        <v>642.37412465037914</v>
+        <f t="shared" si="0"/>
+        <v>642.37412490179906</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.2">
@@ -4454,7 +4499,7 @@
         <v>376.6344466955648</v>
       </c>
       <c r="C34" s="1">
-        <f t="shared" si="0"/>
+        <f>I$5/(SQRT(2*PI())*I$13)*EXP(-(LN(A34/I$9)^2)/(2*I$13^2))+I$6/(SQRT(2*PI())*I$14)*EXP(-(LN(A34/I$10)^2)/(2*I$14^2))+ I$7/(SQRT(2*PI())*I$15)*EXP(-(LN(A34/I$11)^2)/(2*I$15^2))</f>
         <v>346.51013488677359</v>
       </c>
       <c r="D34" s="1">
@@ -4464,8 +4509,8 @@
         <v>561.03433332597172</v>
       </c>
       <c r="F34" s="1">
-        <f t="shared" si="1"/>
-        <v>530.78654172861206</v>
+        <f t="shared" si="0"/>
+        <v>530.78659897571583</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.2">
@@ -4476,7 +4521,7 @@
         <v>255.24642842314179</v>
       </c>
       <c r="C35" s="1">
-        <f t="shared" si="0"/>
+        <f>I$5/(SQRT(2*PI())*I$13)*EXP(-(LN(A35/I$9)^2)/(2*I$13^2))+I$6/(SQRT(2*PI())*I$14)*EXP(-(LN(A35/I$10)^2)/(2*I$14^2))+ I$7/(SQRT(2*PI())*I$15)*EXP(-(LN(A35/I$11)^2)/(2*I$15^2))</f>
         <v>270.10644516484115</v>
       </c>
       <c r="D35" s="1">
@@ -4486,8 +4531,8 @@
         <v>462.22849588417802</v>
       </c>
       <c r="F35" s="1">
-        <f t="shared" si="1"/>
-        <v>428.1462274291045</v>
+        <f t="shared" si="0"/>
+        <v>428.1520780249167</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.2">
@@ -4498,7 +4543,7 @@
         <v>241.98196234508271</v>
       </c>
       <c r="C36" s="1">
-        <f t="shared" si="0"/>
+        <f>I$5/(SQRT(2*PI())*I$13)*EXP(-(LN(A36/I$9)^2)/(2*I$13^2))+I$6/(SQRT(2*PI())*I$14)*EXP(-(LN(A36/I$10)^2)/(2*I$14^2))+ I$7/(SQRT(2*PI())*I$15)*EXP(-(LN(A36/I$11)^2)/(2*I$15^2))</f>
         <v>246.68944948999234</v>
       </c>
       <c r="D36" s="1">
@@ -4508,8 +4553,8 @@
         <v>417.565283330988</v>
       </c>
       <c r="F36" s="1">
-        <f t="shared" si="1"/>
-        <v>403.41660106339543</v>
+        <f t="shared" si="0"/>
+        <v>403.67213727244786</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.2">
@@ -4520,7 +4565,7 @@
         <v>157.73512437240302</v>
       </c>
       <c r="C37" s="1">
-        <f t="shared" si="0"/>
+        <f>I$5/(SQRT(2*PI())*I$13)*EXP(-(LN(A37/I$9)^2)/(2*I$13^2))+I$6/(SQRT(2*PI())*I$14)*EXP(-(LN(A37/I$10)^2)/(2*I$14^2))+ I$7/(SQRT(2*PI())*I$15)*EXP(-(LN(A37/I$11)^2)/(2*I$15^2))</f>
         <v>162.61976469288493</v>
       </c>
       <c r="D37" s="1">
@@ -4530,8 +4575,8 @@
         <v>234.9284858457533</v>
       </c>
       <c r="F37" s="1">
-        <f t="shared" si="1"/>
-        <v>229.62091679840395</v>
+        <f t="shared" si="0"/>
+        <v>234.14276790962415</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.2">
@@ -4542,7 +4587,7 @@
         <v>115.55782817348359</v>
       </c>
       <c r="C38" s="1">
-        <f t="shared" si="0"/>
+        <f>I$5/(SQRT(2*PI())*I$13)*EXP(-(LN(A38/I$9)^2)/(2*I$13^2))+I$6/(SQRT(2*PI())*I$14)*EXP(-(LN(A38/I$10)^2)/(2*I$14^2))+ I$7/(SQRT(2*PI())*I$15)*EXP(-(LN(A38/I$11)^2)/(2*I$15^2))</f>
         <v>86.752788014352063</v>
       </c>
       <c r="D38" s="1">
@@ -4552,8 +4597,8 @@
         <v>163.79350266435569</v>
       </c>
       <c r="F38" s="1">
-        <f t="shared" si="1"/>
-        <v>156.57549736822082</v>
+        <f t="shared" si="0"/>
+        <v>188.84328343322974</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.2">
@@ -4564,7 +4609,7 @@
         <v>43.851103979061016</v>
       </c>
       <c r="C39" s="1">
-        <f t="shared" si="0"/>
+        <f>I$5/(SQRT(2*PI())*I$13)*EXP(-(LN(A39/I$9)^2)/(2*I$13^2))+I$6/(SQRT(2*PI())*I$14)*EXP(-(LN(A39/I$10)^2)/(2*I$14^2))+ I$7/(SQRT(2*PI())*I$15)*EXP(-(LN(A39/I$11)^2)/(2*I$15^2))</f>
         <v>53.464626079080588</v>
       </c>
       <c r="D39" s="1">
@@ -4574,8 +4619,8 @@
         <v>168.64924833160433</v>
       </c>
       <c r="F39" s="1">
-        <f t="shared" si="1"/>
-        <v>101.81140037751567</v>
+        <f t="shared" si="0"/>
+        <v>189.78153820908318</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.2">
@@ -4586,7 +4631,7 @@
         <v>33.978321739525342</v>
       </c>
       <c r="C40" s="1">
-        <f t="shared" si="0"/>
+        <f>I$5/(SQRT(2*PI())*I$13)*EXP(-(LN(A40/I$9)^2)/(2*I$13^2))+I$6/(SQRT(2*PI())*I$14)*EXP(-(LN(A40/I$10)^2)/(2*I$14^2))+ I$7/(SQRT(2*PI())*I$15)*EXP(-(LN(A40/I$11)^2)/(2*I$15^2))</f>
         <v>31.795638351616027</v>
       </c>
       <c r="D40" s="1">
@@ -4596,8 +4641,8 @@
         <v>134.95921943656242</v>
       </c>
       <c r="F40" s="1">
-        <f t="shared" si="1"/>
-        <v>62.707890466235867</v>
+        <f t="shared" si="0"/>
+        <v>150.06106151659179</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.2">
@@ -4608,7 +4653,7 @@
         <v>24.482835800087859</v>
       </c>
       <c r="C41" s="1">
-        <f t="shared" si="0"/>
+        <f>I$5/(SQRT(2*PI())*I$13)*EXP(-(LN(A41/I$9)^2)/(2*I$13^2))+I$6/(SQRT(2*PI())*I$14)*EXP(-(LN(A41/I$10)^2)/(2*I$14^2))+ I$7/(SQRT(2*PI())*I$15)*EXP(-(LN(A41/I$11)^2)/(2*I$15^2))</f>
         <v>17.881837418899167</v>
       </c>
       <c r="D41" s="1">
@@ -4618,8 +4663,8 @@
         <v>62.138519255435824</v>
       </c>
       <c r="F41" s="1">
-        <f t="shared" si="1"/>
-        <v>36.524529466211739</v>
+        <f t="shared" si="0"/>
+        <v>66.771865453561816</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.2">
@@ -4630,7 +4675,7 @@
         <v>5.2543276002820409</v>
       </c>
       <c r="C42" s="1">
-        <f t="shared" si="0"/>
+        <f>I$5/(SQRT(2*PI())*I$13)*EXP(-(LN(A42/I$9)^2)/(2*I$13^2))+I$6/(SQRT(2*PI())*I$14)*EXP(-(LN(A42/I$10)^2)/(2*I$14^2))+ I$7/(SQRT(2*PI())*I$15)*EXP(-(LN(A42/I$11)^2)/(2*I$15^2))</f>
         <v>9.4919207929418583</v>
       </c>
       <c r="D42" s="2">
@@ -4640,8 +4685,8 @@
         <v>28.968435778672355</v>
       </c>
       <c r="F42" s="1">
-        <f t="shared" si="1"/>
-        <v>19.97675800626498</v>
+        <f t="shared" si="0"/>
+        <v>23.400060915912007</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added new project related to cloud seeding
</commit_message>
<xml_diff>
--- a/parcel-modelling/data/Model_inputs_DCMEX.xlsx
+++ b/parcel-modelling/data/Model_inputs_DCMEX.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mccikpc2/Dropbox (Personal)/programming/teaching-repos/projects-and-teaching/parcel-modelling/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{944D647F-4AB6-5642-A7BA-D66989E4297B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{4B2A1776-524F-A047-BBFF-FE1D436B75F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="17280" yWindow="760" windowWidth="17280" windowHeight="20260" xr2:uid="{894127C6-20C5-4B29-9E35-433370B386C8}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="24780" windowHeight="20440" xr2:uid="{894127C6-20C5-4B29-9E35-433370B386C8}"/>
   </bookViews>
   <sheets>
     <sheet name="sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="26">
   <si>
     <t>dN/dlnDp</t>
   </si>
@@ -111,6 +111,9 @@
   </si>
   <si>
     <t>Parameters for Case 2</t>
+  </si>
+  <si>
+    <t>convert to number per kg</t>
   </si>
 </sst>
 </file>
@@ -3537,7 +3540,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0ECA62D5-9912-440B-B476-66EE5BC205DA}">
   <dimension ref="A1:R42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="171" workbookViewId="0">
       <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
@@ -3698,6 +3701,9 @@
         <v>24</v>
       </c>
       <c r="L4" s="11"/>
+      <c r="M4" s="1" t="s">
+        <v>25</v>
+      </c>
       <c r="R4" s="1">
         <f>1/(LOG10(10)/LN(10))</f>
         <v>2.3025850929940459</v>
@@ -3737,6 +3743,14 @@
       <c r="L5" s="11">
         <v>850</v>
       </c>
+      <c r="M5" s="1">
+        <f>I5/(101325/273.15/287)</f>
+        <v>889.74248704663205</v>
+      </c>
+      <c r="N5" s="1">
+        <f>L5/(101325/273.15/287)</f>
+        <v>657.63575129533672</v>
+      </c>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A6">
@@ -3772,6 +3786,14 @@
       <c r="L6" s="11">
         <v>7</v>
       </c>
+      <c r="M6" s="1">
+        <f>I6/(101325/273.15/287)</f>
+        <v>15.473782383419687</v>
+      </c>
+      <c r="N6" s="1">
+        <f>L6/(101325/273.15/287)</f>
+        <v>5.4158238341968907</v>
+      </c>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A7">
@@ -3807,6 +3829,14 @@
       <c r="L7" s="11">
         <v>650</v>
       </c>
+      <c r="M7" s="1">
+        <f>I7/(101325/273.15/287)</f>
+        <v>270.79119170984455</v>
+      </c>
+      <c r="N7" s="1">
+        <f>L7/(101325/273.15/287)</f>
+        <v>502.89792746113983</v>
+      </c>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A8">
@@ -3840,6 +3870,10 @@
       <c r="L8" s="11">
         <v>20</v>
       </c>
+      <c r="N8" s="1">
+        <f>L8/(101325/273.15/287)</f>
+        <v>15.473782383419687</v>
+      </c>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A9">
@@ -3909,6 +3943,14 @@
       </c>
       <c r="L10" s="11">
         <v>0.19500000000000001</v>
+      </c>
+      <c r="M10" s="1">
+        <f>SUM(M5:M7)</f>
+        <v>1176.0074611398963</v>
+      </c>
+      <c r="N10" s="1">
+        <f>SUM(N5:N8)</f>
+        <v>1181.4232849740931</v>
       </c>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.2">

</xml_diff>